<commit_message>
Update Test Bounder Domain
</commit_message>
<xml_diff>
--- a/app/Test/Test Bounder Domain.xlsx
+++ b/app/Test/Test Bounder Domain.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="19395" windowHeight="7155"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="19395" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Visit" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>valid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -183,6 +183,110 @@
   </si>
   <si>
     <t>Add/update patient</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add/Update Visit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anything</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chief Complaint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-255</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight(kg)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>others</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes, No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height(inch)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Height(cm)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1c(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">3--20 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>letters, signs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>61-?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number in format 9'2''</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8,8'''</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight/Weight goal(lb)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all the allegies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes, No, Unknown</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -235,7 +339,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -247,6 +351,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -291,6 +401,102 @@
   <autoFilter ref="A50:C52"/>
   <tableColumns count="3">
     <tableColumn id="1" name="ZIP"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="表2_14" displayName="表2_14" ref="A3:C5" totalsRowShown="0">
+  <autoFilter ref="A3:C5"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Chief Complaint"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="表2_1415" displayName="表2_1415" ref="A8:C10" totalsRowShown="0">
+  <autoFilter ref="A8:C10"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Weight/Weight goal(lb)"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="表2_141516" displayName="表2_141516" ref="A12:C14" totalsRowShown="0">
+  <autoFilter ref="A12:C14"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Weight(kg)"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_1415162" displayName="表2_1415162" ref="A35:C36" totalsRowShown="0">
+  <autoFilter ref="A35:C36"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="others"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="表2_14151617" displayName="表2_14151617" ref="A17:C19" totalsRowShown="0">
+  <autoFilter ref="A17:C19"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Height(inch)"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="表2_1415161718" displayName="表2_1415161718" ref="A21:C23" totalsRowShown="0">
+  <autoFilter ref="A21:C23"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Height(cm)"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="表2_141516171819" displayName="表2_141516171819" ref="A26:C28" totalsRowShown="0">
+  <autoFilter ref="A26:C28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="A1c(%)"/>
+    <tableColumn id="2" name="valid"/>
+    <tableColumn id="3" name="invalid"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="表2_141516220" displayName="表2_141516220" ref="A31:C32" totalsRowShown="0">
+  <autoFilter ref="A31:C32"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="all the allegies"/>
     <tableColumn id="2" name="valid"/>
     <tableColumn id="3" name="invalid"/>
   </tableColumns>
@@ -684,7 +890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1084,7 +1292,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1096,13 +1304,272 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="8">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>